<commit_message>
feat: using try catch, formulate msg from app
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_out.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_out.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -940,23 +940,9 @@
         <v>f530107653ea3ae4c621abfb444fe4b99b120b5918aa7d39fae13971c4a51b4b</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Thu Feb 02 2023 08:47:16 GMT+0000 (Coordinated Universal Time)</v>
-      </c>
-      <c r="C41" t="str">
-        <v>commemt: a test case for DR update, file hash: https://github.com/tibonto/dr/archive/08cc171ae8fe31f2c84c826b4cc42f722158e303.zip</v>
-      </c>
-      <c r="D41" t="str">
-        <v>bf197c4de57709866be230d1a0ae05577d3bf7aed75287414b79fd576bec53d0</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D40"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>